<commit_message>
updated cnert excel sheet
</commit_message>
<xml_diff>
--- a/speed_up_cnert_paper.xlsx
+++ b/speed_up_cnert_paper.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Factor-Graph-Implementation-Final-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhargav04\Documents\distributed computing group 6\Factor-Graph-Implementation-Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{798D4D5F-F24D-41CC-9A69-07D38C62D3CA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6AE9BF1-1EF0-4DBF-9B7C-670446CE6A41}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" tabRatio="368" xr2:uid="{CE8E9581-15FF-4D4F-942C-DB66E5108511}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -46,9 +52,6 @@
   </si>
   <si>
     <t>#decoding_iterations = 10</t>
-  </si>
-  <si>
-    <t>#times_run = 50</t>
   </si>
   <si>
     <t>#ones_per_row = 12</t>
@@ -79,6 +82,9 @@
   </si>
   <si>
     <t>(The number of processors (#Procs) are on a per server basis)</t>
+  </si>
+  <si>
+    <t>#num_vectors = 1000</t>
   </si>
 </sst>
 </file>
@@ -432,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{024FF512-29FA-4737-8156-DF564DC3DDD7}">
   <dimension ref="A1:M109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H104" sqref="H104"/>
+    <sheetView tabSelected="1" topLeftCell="G14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,7 +451,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -453,21 +459,21 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
       <c r="J4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -475,7 +481,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -487,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J5" t="s">
         <v>4</v>
@@ -530,17 +536,17 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>3.2486000000000001E-2</v>
+        <v>0.64725100000000002</v>
       </c>
       <c r="D7">
-        <v>1.7874650000000001</v>
+        <v>35.27084</v>
       </c>
       <c r="E7">
-        <f>$C$7/C7</f>
+        <f t="shared" ref="E7:E13" si="0">$C$7/C7</f>
         <v>1</v>
       </c>
       <c r="F7">
-        <f>$D$7/D7</f>
+        <f t="shared" ref="F7:F13" si="1">$D$7/D7</f>
         <v>1</v>
       </c>
       <c r="H7">
@@ -550,10 +556,10 @@
         <v>1</v>
       </c>
       <c r="J7">
-        <v>1.9520690000000001</v>
+        <v>0.65088699999999999</v>
       </c>
       <c r="K7">
-        <v>105.999876</v>
+        <v>34.933281999999998</v>
       </c>
       <c r="L7">
         <f>$J$7/J7</f>
@@ -569,35 +575,35 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>1.7191999999999999E-2</v>
+        <v>0.33466099999999999</v>
       </c>
       <c r="D8">
-        <v>2.369621</v>
+        <v>50.236573999999997</v>
       </c>
       <c r="E8">
-        <f>$C$7/C8</f>
-        <v>1.889599813866915</v>
+        <f t="shared" si="0"/>
+        <v>1.9340496801240661</v>
       </c>
       <c r="F8">
-        <f>$D$7/D8</f>
-        <v>0.75432526973722802</v>
+        <f t="shared" si="1"/>
+        <v>0.70209485224848334</v>
       </c>
       <c r="I8">
         <v>2</v>
       </c>
       <c r="J8">
-        <v>0.98807999999999996</v>
+        <v>0.35188199999999997</v>
       </c>
       <c r="K8">
-        <v>53.960945000000002</v>
+        <v>17.714580000000002</v>
       </c>
       <c r="L8">
-        <f t="shared" ref="L8:L13" si="0">$J$7/J8</f>
-        <v>1.9756183709821069</v>
+        <f t="shared" ref="L8:L13" si="2">$J$7/J8</f>
+        <v>1.8497308756912829</v>
       </c>
       <c r="M8">
-        <f t="shared" ref="M8:M13" si="1">$K$7/K8</f>
-        <v>1.9643813873163265</v>
+        <f t="shared" ref="M8:M13" si="3">$K$7/K8</f>
+        <v>1.972007352135924</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -605,35 +611,35 @@
         <v>4</v>
       </c>
       <c r="C9">
-        <v>9.41E-3</v>
+        <v>0.18406900000000001</v>
       </c>
       <c r="D9">
-        <v>2.0163489999999999</v>
+        <v>40.549596000000001</v>
       </c>
       <c r="E9">
-        <f>$C$7/C9</f>
-        <v>3.4522848034006377</v>
+        <f t="shared" si="0"/>
+        <v>3.5163498470682191</v>
       </c>
       <c r="F9">
-        <f>$D$7/D9</f>
-        <v>0.8864859208400927</v>
+        <f t="shared" si="1"/>
+        <v>0.86981976343241496</v>
       </c>
       <c r="I9">
         <v>4</v>
       </c>
       <c r="J9">
-        <v>0.54756899999999997</v>
+        <v>0.182946</v>
       </c>
       <c r="K9">
-        <v>28.524149000000001</v>
+        <v>9.1029499999999999</v>
       </c>
       <c r="L9">
-        <f t="shared" si="0"/>
-        <v>3.5649735467128347</v>
+        <f t="shared" si="2"/>
+        <v>3.5578094082406833</v>
       </c>
       <c r="M9">
-        <f t="shared" si="1"/>
-        <v>3.7161450811380909</v>
+        <f t="shared" si="3"/>
+        <v>3.8375781477433137</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -641,35 +647,35 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>8.1519999999999995E-3</v>
+        <v>0.11362700000000001</v>
       </c>
       <c r="D10">
-        <v>1.4840409999999999</v>
+        <v>28.973956000000001</v>
       </c>
       <c r="E10">
-        <f>$C$7/C10</f>
-        <v>3.9850343473994116</v>
+        <f t="shared" si="0"/>
+        <v>5.696278173321482</v>
       </c>
       <c r="F10">
-        <f>$D$7/D10</f>
-        <v>1.204457963088621</v>
+        <f t="shared" si="1"/>
+        <v>1.2173291075612871</v>
       </c>
       <c r="I10">
         <v>8</v>
       </c>
       <c r="J10">
-        <v>0.30534699999999998</v>
+        <v>0.10628</v>
       </c>
       <c r="K10">
-        <v>14.934621</v>
+        <v>5.6964290000000002</v>
       </c>
       <c r="L10">
-        <f t="shared" si="0"/>
-        <v>6.3929529355127119</v>
+        <f t="shared" si="2"/>
+        <v>6.1242660895747081</v>
       </c>
       <c r="M10">
-        <f t="shared" si="1"/>
-        <v>7.0975939730911151</v>
+        <f t="shared" si="3"/>
+        <v>6.1324879147971467</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -677,35 +683,35 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <v>7.9939999999999994E-3</v>
+        <v>8.6116999999999999E-2</v>
       </c>
       <c r="D11">
-        <v>1.121132</v>
+        <v>21.764606000000001</v>
       </c>
       <c r="E11">
-        <f>$C$7/C11</f>
-        <v>4.0637978483862902</v>
+        <f t="shared" si="0"/>
+        <v>7.5159492318589827</v>
       </c>
       <c r="F11">
-        <f>$D$7/D11</f>
-        <v>1.5943394711773458</v>
+        <f t="shared" si="1"/>
+        <v>1.620559545162453</v>
       </c>
       <c r="I11">
         <v>16</v>
       </c>
       <c r="J11">
-        <v>0.20094500000000001</v>
+        <v>6.6230999999999998E-2</v>
       </c>
       <c r="K11">
-        <v>8.5929339999999996</v>
+        <v>2.9151669999999998</v>
       </c>
       <c r="L11">
-        <f t="shared" si="0"/>
-        <v>9.7144442509144291</v>
+        <f t="shared" si="2"/>
+        <v>9.8275278947924694</v>
       </c>
       <c r="M11">
-        <f t="shared" si="1"/>
-        <v>12.335702334033988</v>
+        <f t="shared" si="3"/>
+        <v>11.98328672079507</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -713,35 +719,35 @@
         <v>32</v>
       </c>
       <c r="C12">
-        <v>1.6102000000000002E-2</v>
+        <v>9.3309000000000003E-2</v>
       </c>
       <c r="D12">
-        <v>0.86814999999999998</v>
+        <v>17.424378000000001</v>
       </c>
       <c r="E12">
-        <f>$C$7/C12</f>
-        <v>2.0175133523785864</v>
+        <f t="shared" si="0"/>
+        <v>6.9366406241627283</v>
       </c>
       <c r="F12">
-        <f>$D$7/D12</f>
-        <v>2.0589356677993438</v>
+        <f t="shared" si="1"/>
+        <v>2.0242237628224089</v>
       </c>
       <c r="I12">
         <v>32</v>
       </c>
       <c r="J12">
-        <v>0.19093299999999999</v>
+        <v>5.3786E-2</v>
       </c>
       <c r="K12">
-        <v>5.4774700000000003</v>
+        <v>1.5224610000000001</v>
       </c>
       <c r="L12">
-        <f t="shared" si="0"/>
-        <v>10.22384291872018</v>
+        <f t="shared" si="2"/>
+        <v>12.101420443981706</v>
       </c>
       <c r="M12">
-        <f t="shared" si="1"/>
-        <v>19.351977464048183</v>
+        <f t="shared" si="3"/>
+        <v>22.945272161323015</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -749,35 +755,35 @@
         <v>64</v>
       </c>
       <c r="C13">
-        <v>1.5474999999999999E-2</v>
+        <v>0.182697</v>
       </c>
       <c r="D13">
-        <v>0.91809700000000005</v>
+        <v>17.088065</v>
       </c>
       <c r="E13">
-        <f>$C$7/C13</f>
-        <v>2.0992568659127628</v>
+        <f t="shared" si="0"/>
+        <v>3.542756586041369</v>
       </c>
       <c r="F13">
-        <f>$D$7/D13</f>
-        <v>1.9469239089115855</v>
+        <f t="shared" si="1"/>
+        <v>2.0640628415212605</v>
       </c>
       <c r="I13">
         <v>64</v>
       </c>
       <c r="J13">
-        <v>0.230074</v>
+        <v>9.0401999999999996E-2</v>
       </c>
       <c r="K13">
-        <v>3.806727</v>
+        <v>1.2827710000000001</v>
       </c>
       <c r="L13">
-        <f t="shared" si="0"/>
-        <v>8.484526717490894</v>
+        <f t="shared" si="2"/>
+        <v>7.1999181434039068</v>
       </c>
       <c r="M13">
-        <f t="shared" si="1"/>
-        <v>27.845410506190753</v>
+        <f t="shared" si="3"/>
+        <v>27.232672082546298</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -788,10 +794,10 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>4.3534000000000003E-2</v>
+        <v>0.83038299999999998</v>
       </c>
       <c r="D14">
-        <v>1.1834309999999999</v>
+        <v>23.253250999999999</v>
       </c>
       <c r="E14">
         <f>$C$14/C14</f>
@@ -808,10 +814,10 @@
         <v>1</v>
       </c>
       <c r="J14">
-        <v>2.50922</v>
+        <v>0.84937700000000005</v>
       </c>
       <c r="K14">
-        <v>69.548351999999994</v>
+        <v>23.107415</v>
       </c>
       <c r="L14">
         <f>$J$14/J14</f>
@@ -827,35 +833,35 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <v>2.2783999999999999E-2</v>
+        <v>0.44527499999999998</v>
       </c>
       <c r="D15">
-        <v>1.5639620000000001</v>
+        <v>32.044347999999999</v>
       </c>
       <c r="E15">
-        <f t="shared" ref="E15:E20" si="2">$C$14/C15</f>
-        <v>1.9107268258426968</v>
+        <f t="shared" ref="E15:E20" si="4">$C$14/C15</f>
+        <v>1.86487676155185</v>
       </c>
       <c r="F15">
-        <f t="shared" ref="F15:F20" si="3">$D$14/D15</f>
-        <v>0.75668782233839427</v>
+        <f t="shared" ref="F15:F20" si="5">$D$14/D15</f>
+        <v>0.72565842188457075</v>
       </c>
       <c r="I15">
         <v>2</v>
       </c>
       <c r="J15">
-        <v>1.3166199999999999</v>
+        <v>0.45709</v>
       </c>
       <c r="K15">
-        <v>35.056322000000002</v>
+        <v>11.827881</v>
       </c>
       <c r="L15">
-        <f t="shared" ref="L15:L20" si="4">$J$14/J15</f>
-        <v>1.9058042563533899</v>
+        <f t="shared" ref="L15:L20" si="6">$J$14/J15</f>
+        <v>1.8582270450020786</v>
       </c>
       <c r="M15">
-        <f t="shared" ref="M15:M20" si="5">$K$14/K15</f>
-        <v>1.9839032742796003</v>
+        <f t="shared" ref="M15:M20" si="7">$K$14/K15</f>
+        <v>1.95363945579094</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -863,35 +869,35 @@
         <v>4</v>
       </c>
       <c r="C16">
-        <v>1.2355E-2</v>
+        <v>0.236739</v>
       </c>
       <c r="D16">
-        <v>1.355227</v>
+        <v>27.556137</v>
       </c>
       <c r="E16">
-        <f t="shared" si="2"/>
-        <v>3.5235936867664917</v>
+        <f t="shared" si="4"/>
+        <v>3.5075885257604367</v>
       </c>
       <c r="F16">
-        <f t="shared" si="3"/>
-        <v>0.8732345208588671</v>
+        <f>$D$14/D16</f>
+        <v>0.84385017391951556</v>
       </c>
       <c r="I16">
         <v>4</v>
       </c>
       <c r="J16">
-        <v>0.69020300000000001</v>
+        <v>0.23291300000000001</v>
       </c>
       <c r="K16">
-        <v>18.108908</v>
+        <v>5.9464170000000003</v>
       </c>
       <c r="L16">
-        <f t="shared" si="4"/>
-        <v>3.6354811555440936</v>
+        <f t="shared" si="6"/>
+        <v>3.6467565142349292</v>
       </c>
       <c r="M16">
-        <f t="shared" si="5"/>
-        <v>3.8405602369839196</v>
+        <f t="shared" si="7"/>
+        <v>3.8859392134793103</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -899,35 +905,35 @@
         <v>8</v>
       </c>
       <c r="C17">
-        <v>9.2289999999999994E-3</v>
+        <v>0.14535300000000001</v>
       </c>
       <c r="D17">
-        <v>1.016797</v>
+        <v>20.046272999999999</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
-        <v>4.7170874417596709</v>
+        <f t="shared" si="4"/>
+        <v>5.7128714233624347</v>
       </c>
       <c r="F17">
-        <f t="shared" si="3"/>
-        <v>1.1638812860384127</v>
+        <f t="shared" si="5"/>
+        <v>1.1599787651300568</v>
       </c>
       <c r="I17">
         <v>8</v>
       </c>
       <c r="J17">
-        <v>0.41352899999999998</v>
+        <v>0.134187</v>
       </c>
       <c r="K17">
-        <v>9.9828840000000003</v>
+        <v>3.8214459999999999</v>
       </c>
       <c r="L17">
-        <f t="shared" si="4"/>
-        <v>6.0678211201632779</v>
+        <f t="shared" si="6"/>
+        <v>6.3298009494213305</v>
       </c>
       <c r="M17">
-        <f t="shared" si="5"/>
-        <v>6.9667595055697324</v>
+        <f t="shared" si="7"/>
+        <v>6.046772609111839</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -935,35 +941,35 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <v>9.4560000000000009E-3</v>
+        <v>0.107465</v>
       </c>
       <c r="D18">
-        <v>0.76556900000000006</v>
+        <v>15.126096</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
-        <v>4.603849407783418</v>
+        <f t="shared" si="4"/>
+        <v>7.7270087935606933</v>
       </c>
       <c r="F18">
-        <f t="shared" si="3"/>
-        <v>1.5458188615265245</v>
+        <f t="shared" si="5"/>
+        <v>1.5372936281774225</v>
       </c>
       <c r="I18">
         <v>16</v>
       </c>
       <c r="J18">
-        <v>0.39608100000000002</v>
+        <v>8.3541000000000004E-2</v>
       </c>
       <c r="K18">
-        <v>8.0224410000000006</v>
+        <v>1.885529</v>
       </c>
       <c r="L18">
-        <f t="shared" si="4"/>
-        <v>6.3351183217574176</v>
+        <f t="shared" si="6"/>
+        <v>10.167187369076261</v>
       </c>
       <c r="M18">
-        <f t="shared" si="5"/>
-        <v>8.6692257381512672</v>
+        <f t="shared" si="7"/>
+        <v>12.25513635695871</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -971,35 +977,35 @@
         <v>32</v>
       </c>
       <c r="C19">
-        <v>1.3282E-2</v>
+        <v>0.12815299999999999</v>
       </c>
       <c r="D19">
-        <v>0.62478699999999998</v>
+        <v>11.913065</v>
       </c>
       <c r="E19">
-        <f t="shared" si="2"/>
-        <v>3.2776690257491343</v>
+        <f t="shared" si="4"/>
+        <v>6.479622014311019</v>
       </c>
       <c r="F19">
-        <f t="shared" si="3"/>
-        <v>1.8941351212493216</v>
+        <f t="shared" si="5"/>
+        <v>1.951911703663163</v>
       </c>
       <c r="I19">
         <v>32</v>
       </c>
       <c r="J19">
-        <v>0.26988299999999998</v>
+        <v>9.4918000000000002E-2</v>
       </c>
       <c r="K19">
-        <v>4.337218</v>
+        <v>1.433011</v>
       </c>
       <c r="L19">
-        <f t="shared" si="4"/>
-        <v>9.2974362964692112</v>
+        <f t="shared" si="6"/>
+        <v>8.948534524536969</v>
       </c>
       <c r="M19">
-        <f t="shared" si="5"/>
-        <v>16.035244712163419</v>
+        <f t="shared" si="7"/>
+        <v>16.12507859325574</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1007,35 +1013,35 @@
         <v>64</v>
       </c>
       <c r="C20">
-        <v>1.8804999999999999E-2</v>
+        <v>0.199985</v>
       </c>
       <c r="D20">
-        <v>0.66095300000000001</v>
+        <v>12.383607</v>
       </c>
       <c r="E20">
-        <f t="shared" si="2"/>
-        <v>2.3150226003722416</v>
+        <f t="shared" si="4"/>
+        <v>4.1522264169812733</v>
       </c>
       <c r="F20">
-        <f t="shared" si="3"/>
-        <v>1.7904919109225617</v>
+        <f t="shared" si="5"/>
+        <v>1.8777445860483137</v>
       </c>
       <c r="I20">
         <v>64</v>
       </c>
       <c r="J20">
-        <v>0.26486799999999999</v>
+        <v>9.3269000000000005E-2</v>
       </c>
       <c r="K20">
-        <v>2.3457050000000002</v>
+        <v>0.786721</v>
       </c>
       <c r="L20">
-        <f t="shared" si="4"/>
-        <v>9.4734735792923264</v>
+        <f t="shared" si="6"/>
+        <v>9.1067450063793967</v>
       </c>
       <c r="M20">
-        <f t="shared" si="5"/>
-        <v>29.649232107191651</v>
+        <f t="shared" si="7"/>
+        <v>29.371803981335187</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1046,10 +1052,10 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>3.2113999999999997E-2</v>
+        <v>0.65215900000000004</v>
       </c>
       <c r="D21">
-        <v>0.57597600000000004</v>
+        <v>11.602683000000001</v>
       </c>
       <c r="E21">
         <f>$C$21/C21</f>
@@ -1066,10 +1072,10 @@
         <v>1</v>
       </c>
       <c r="J21">
-        <v>1.9301950000000001</v>
+        <v>0.65266500000000005</v>
       </c>
       <c r="K21">
-        <v>35.068238999999998</v>
+        <v>11.534471999999999</v>
       </c>
       <c r="L21">
         <f>$J$21/J21</f>
@@ -1085,35 +1091,35 @@
         <v>2</v>
       </c>
       <c r="C22">
-        <v>1.7295999999999999E-2</v>
+        <v>0.32833699999999999</v>
       </c>
       <c r="D22">
-        <v>0.75096499999999999</v>
+        <v>14.643274999999999</v>
       </c>
       <c r="E22">
-        <f t="shared" ref="E22:E27" si="6">$C$21/C22</f>
-        <v>1.8567298797409806</v>
+        <f t="shared" ref="E22:E27" si="8">$C$21/C22</f>
+        <v>1.9862488845302237</v>
       </c>
       <c r="F22">
-        <f t="shared" ref="F22:F27" si="7">$D$21/D22</f>
-        <v>0.76698115091915076</v>
+        <f t="shared" ref="F22:F27" si="9">$D$21/D22</f>
+        <v>0.79235574009229504</v>
       </c>
       <c r="I22">
         <v>2</v>
       </c>
       <c r="J22">
-        <v>1.0159469999999999</v>
+        <v>0.34576099999999999</v>
       </c>
       <c r="K22">
-        <v>17.465012000000002</v>
+        <v>5.8460479999999997</v>
       </c>
       <c r="L22">
-        <f t="shared" ref="L22:L27" si="8">$J$21/J22</f>
-        <v>1.899897337164242</v>
+        <f t="shared" ref="L22:L27" si="10">$J$21/J22</f>
+        <v>1.8876189043877132</v>
       </c>
       <c r="M22">
-        <f t="shared" ref="M22:M27" si="9">$K$21/K22</f>
-        <v>2.0079138222178146</v>
+        <f t="shared" ref="M22:M27" si="11">$K$21/K22</f>
+        <v>1.9730375118370564</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1121,35 +1127,35 @@
         <v>4</v>
       </c>
       <c r="C23">
-        <v>1.0085999999999999E-2</v>
+        <v>0.19453999999999999</v>
       </c>
       <c r="D23">
-        <v>0.70815799999999995</v>
+        <v>14.899122</v>
       </c>
       <c r="E23">
-        <f t="shared" si="6"/>
-        <v>3.1840174499305967</v>
+        <f t="shared" si="8"/>
+        <v>3.3523131489667937</v>
       </c>
       <c r="F23">
-        <f t="shared" si="7"/>
-        <v>0.81334391477608114</v>
+        <f t="shared" si="9"/>
+        <v>0.77874944577271066</v>
       </c>
       <c r="I23">
         <v>4</v>
       </c>
       <c r="J23">
-        <v>0.53879900000000003</v>
+        <v>0.17966799999999999</v>
       </c>
       <c r="K23">
-        <v>9.0968870000000006</v>
+        <v>3.1393499999999999</v>
       </c>
       <c r="L23">
-        <f t="shared" si="8"/>
-        <v>3.5824027141846959</v>
+        <f t="shared" si="10"/>
+        <v>3.6326168265912688</v>
       </c>
       <c r="M23">
-        <f t="shared" si="9"/>
-        <v>3.8549713764719731</v>
+        <f t="shared" si="11"/>
+        <v>3.67415930049214</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1157,35 +1163,35 @@
         <v>8</v>
       </c>
       <c r="C24">
-        <v>6.9470000000000001E-3</v>
+        <v>0.118118</v>
       </c>
       <c r="D24">
-        <v>0.56173799999999996</v>
+        <v>11.065439</v>
       </c>
       <c r="E24">
-        <f t="shared" si="6"/>
-        <v>4.6227148409385341</v>
+        <f t="shared" si="8"/>
+        <v>5.5212499365041738</v>
       </c>
       <c r="F24">
-        <f t="shared" si="7"/>
-        <v>1.0253463358362798</v>
+        <f t="shared" si="9"/>
+        <v>1.0485515305809376</v>
       </c>
       <c r="I24">
         <v>8</v>
       </c>
       <c r="J24">
-        <v>0.30629099999999998</v>
+        <v>0.112235</v>
       </c>
       <c r="K24">
-        <v>5.0019070000000001</v>
+        <v>1.669</v>
       </c>
       <c r="L24">
-        <f t="shared" si="8"/>
-        <v>6.3018338769340279</v>
+        <f t="shared" si="10"/>
+        <v>5.8151646099701519</v>
       </c>
       <c r="M24">
-        <f t="shared" si="9"/>
-        <v>7.0109738145871159</v>
+        <f t="shared" si="11"/>
+        <v>6.9110077890952661</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -1193,35 +1199,35 @@
         <v>16</v>
       </c>
       <c r="C25">
-        <v>7.1209999999999997E-3</v>
+        <v>9.1335E-2</v>
       </c>
       <c r="D25">
-        <v>0.42017599999999999</v>
+        <v>8.4383110000000006</v>
       </c>
       <c r="E25">
-        <f t="shared" si="6"/>
-        <v>4.5097598651874735</v>
+        <f t="shared" si="8"/>
+        <v>7.1402967099140531</v>
       </c>
       <c r="F25">
-        <f t="shared" si="7"/>
-        <v>1.3707969993526523</v>
+        <f t="shared" si="9"/>
+        <v>1.3750006369758119</v>
       </c>
       <c r="I25">
         <v>16</v>
       </c>
       <c r="J25">
-        <v>0.201628</v>
+        <v>6.8117999999999998E-2</v>
       </c>
       <c r="K25">
-        <v>2.813158</v>
+        <v>0.96030000000000004</v>
       </c>
       <c r="L25">
-        <f t="shared" si="8"/>
-        <v>9.5730503699882963</v>
+        <f t="shared" si="10"/>
+        <v>9.5813881793358586</v>
       </c>
       <c r="M25">
-        <f t="shared" si="9"/>
-        <v>12.465790758997539</v>
+        <f t="shared" si="11"/>
+        <v>12.01132146204311</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -1229,35 +1235,35 @@
         <v>32</v>
       </c>
       <c r="C26">
-        <v>1.3428000000000001E-2</v>
+        <v>0.17962800000000001</v>
       </c>
       <c r="D26">
-        <v>0.38878499999999999</v>
+        <v>7.5309189999999999</v>
       </c>
       <c r="E26">
-        <f t="shared" si="6"/>
-        <v>2.3915698540363417</v>
+        <f t="shared" si="8"/>
+        <v>3.6306088137706816</v>
       </c>
       <c r="F26">
-        <f t="shared" si="7"/>
-        <v>1.4814769088313593</v>
+        <f t="shared" si="9"/>
+        <v>1.5406729245129314</v>
       </c>
       <c r="I26">
         <v>32</v>
       </c>
       <c r="J26">
-        <v>0.38315700000000003</v>
+        <v>0.14349999999999999</v>
       </c>
       <c r="K26">
-        <v>2.215554</v>
+        <v>0.72696300000000003</v>
       </c>
       <c r="L26">
-        <f t="shared" si="8"/>
-        <v>5.0376086043058068</v>
+        <f t="shared" si="10"/>
+        <v>4.5481881533101056</v>
       </c>
       <c r="M26">
-        <f t="shared" si="9"/>
-        <v>15.828203239460649</v>
+        <f t="shared" si="11"/>
+        <v>15.866656212214375</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -1265,48 +1271,48 @@
         <v>64</v>
       </c>
       <c r="C27">
-        <v>2.0965999999999999E-2</v>
+        <v>0.23555699999999999</v>
       </c>
       <c r="D27">
-        <v>0.43507499999999999</v>
+        <v>7.8879200000000003</v>
       </c>
       <c r="E27">
-        <f t="shared" si="6"/>
-        <v>1.5317180196508633</v>
+        <f t="shared" si="8"/>
+        <v>2.7685825511447337</v>
       </c>
       <c r="F27">
-        <f t="shared" si="7"/>
-        <v>1.3238545078434754</v>
+        <f t="shared" si="9"/>
+        <v>1.4709432904999038</v>
       </c>
       <c r="I27">
         <v>64</v>
       </c>
       <c r="J27">
-        <v>0.32422800000000002</v>
+        <v>0.110747</v>
       </c>
       <c r="K27">
-        <v>1.199527</v>
+        <v>0.39980199999999999</v>
       </c>
       <c r="L27">
-        <f t="shared" si="8"/>
-        <v>5.9532026845306394</v>
+        <f t="shared" si="10"/>
+        <v>5.8932973353680014</v>
       </c>
       <c r="M27">
-        <f t="shared" si="9"/>
-        <v>29.23505598456725</v>
+        <f t="shared" si="11"/>
+        <v>28.850460978184199</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -1362,11 +1368,11 @@
         <v>0.33839000000000002</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E39" si="10">$C$33/C34</f>
+        <f t="shared" ref="E34:E39" si="12">$C$33/C34</f>
         <v>1.505759162303665</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34:F39" si="11">$D$33/D34</f>
+        <f t="shared" ref="F34:F39" si="13">$D$33/D34</f>
         <v>0.81487632613256888</v>
       </c>
     </row>
@@ -1381,11 +1387,11 @@
         <v>0.294487</v>
       </c>
       <c r="E35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.8341836734693879</v>
       </c>
       <c r="F35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.93636051846091672</v>
       </c>
     </row>
@@ -1400,11 +1406,11 @@
         <v>0.23300899999999999</v>
       </c>
       <c r="E36">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.5537547271745002</v>
       </c>
       <c r="F36">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.1834135162161119</v>
       </c>
     </row>
@@ -1419,11 +1425,11 @@
         <v>0.13514799999999999</v>
       </c>
       <c r="E37">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.347072599531616</v>
       </c>
       <c r="F37">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2.0403261609494776</v>
       </c>
     </row>
@@ -1438,11 +1444,11 @@
         <v>0.14555799999999999</v>
       </c>
       <c r="E38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.64484304932735426</v>
       </c>
       <c r="F38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.8944063534810867</v>
       </c>
     </row>
@@ -1457,11 +1463,11 @@
         <v>0.14627000000000001</v>
       </c>
       <c r="E39">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.5955975921229571E-2</v>
       </c>
       <c r="F39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.8851849319751144</v>
       </c>
     </row>
@@ -1498,11 +1504,11 @@
         <v>1.5639620000000001</v>
       </c>
       <c r="E41">
-        <f t="shared" ref="E41:E46" si="12">$C$40/C41</f>
+        <f t="shared" ref="E41:E46" si="14">$C$40/C41</f>
         <v>1.9107268258426968</v>
       </c>
       <c r="F41">
-        <f t="shared" ref="F41:F46" si="13">$D$40/D41</f>
+        <f t="shared" ref="F41:F46" si="15">$D$40/D41</f>
         <v>0.75668782233839427</v>
       </c>
     </row>
@@ -1517,11 +1523,11 @@
         <v>1.355227</v>
       </c>
       <c r="E42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>3.5235936867664917</v>
       </c>
       <c r="F42">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.8732345208588671</v>
       </c>
     </row>
@@ -1536,11 +1542,11 @@
         <v>1.016797</v>
       </c>
       <c r="E43">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>4.7170874417596709</v>
       </c>
       <c r="F43">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.1638812860384127</v>
       </c>
     </row>
@@ -1555,11 +1561,11 @@
         <v>0.76556900000000006</v>
       </c>
       <c r="E44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>4.603849407783418</v>
       </c>
       <c r="F44">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.5458188615265245</v>
       </c>
     </row>
@@ -1574,11 +1580,11 @@
         <v>0.62478699999999998</v>
       </c>
       <c r="E45">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>3.2776690257491343</v>
       </c>
       <c r="F45">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.8941351212493216</v>
       </c>
     </row>
@@ -1593,17 +1599,17 @@
         <v>0.66095300000000001</v>
       </c>
       <c r="E46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2.3150226003722416</v>
       </c>
       <c r="F46">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.7904919109225617</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1639,11 +1645,11 @@
         <v>0.35753499999999999</v>
       </c>
       <c r="E49">
-        <f t="shared" ref="E49:E54" si="14">$C$48/C49</f>
+        <f t="shared" ref="E49:E54" si="16">$C$48/C49</f>
         <v>1.6229954335091252</v>
       </c>
       <c r="F49">
-        <f t="shared" ref="F49:F54" si="15">$D$48/D49</f>
+        <f t="shared" ref="F49:F54" si="17">$D$48/D49</f>
         <v>0.82151397765253753</v>
       </c>
     </row>
@@ -1658,11 +1664,11 @@
         <v>0.33961400000000003</v>
       </c>
       <c r="E50">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>3.1836771625045244</v>
       </c>
       <c r="F50">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0.8648642282120288</v>
       </c>
     </row>
@@ -1677,11 +1683,11 @@
         <v>0.25603599999999999</v>
       </c>
       <c r="E51">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>6.1722605543211326</v>
       </c>
       <c r="F51">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1.1471824274711369</v>
       </c>
     </row>
@@ -1696,11 +1702,11 @@
         <v>0.194629</v>
       </c>
       <c r="E52">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>9.9461038349194393</v>
       </c>
       <c r="F52">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1.50912762229678</v>
       </c>
     </row>
@@ -1715,11 +1721,11 @@
         <v>0.16245100000000001</v>
       </c>
       <c r="E53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>15.94772624263484</v>
       </c>
       <c r="F53">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1.8080528897944608</v>
       </c>
     </row>
@@ -1734,25 +1740,25 @@
         <v>0.18986800000000001</v>
       </c>
       <c r="E54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>10.088693491350472</v>
       </c>
       <c r="F54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1.5469694735289778</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>15</v>
+      </c>
+      <c r="B57" t="s">
         <v>16</v>
-      </c>
-      <c r="B57" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E58" t="s">
         <v>6</v>
@@ -1760,21 +1766,21 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60" t="s">
+        <v>17</v>
+      </c>
+      <c r="H60" t="s">
         <v>14</v>
       </c>
-      <c r="C60" t="s">
-        <v>7</v>
-      </c>
-      <c r="H60" t="s">
-        <v>15</v>
-      </c>
       <c r="J60" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -1782,7 +1788,7 @@
         <v>0</v>
       </c>
       <c r="B61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C61" t="s">
         <v>4</v>
@@ -1794,7 +1800,7 @@
         <v>0</v>
       </c>
       <c r="I61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J61" t="s">
         <v>4</v>
@@ -1837,18 +1843,18 @@
         <v>1</v>
       </c>
       <c r="C63">
-        <v>2.2407E-2</v>
+        <v>0.41491400000000001</v>
       </c>
       <c r="D63">
-        <v>12.666672</v>
+        <v>260.892695</v>
       </c>
       <c r="E63">
         <f>$C$7/C63</f>
-        <v>1.4498147900209757</v>
+        <v>1.5599642335520132</v>
       </c>
       <c r="F63">
         <f>$D$7/D63</f>
-        <v>0.14111559847764274</v>
+        <v>0.1351928999008577</v>
       </c>
       <c r="H63">
         <v>0.25</v>
@@ -1857,18 +1863,18 @@
         <v>1</v>
       </c>
       <c r="J63">
-        <v>1.053904</v>
+        <v>0.34814299999999998</v>
       </c>
       <c r="K63">
-        <v>52.956316999999999</v>
+        <v>17.903811999999999</v>
       </c>
       <c r="L63">
         <f>$J$7/J63</f>
-        <v>1.852226578511895</v>
+        <v>1.8695966887169928</v>
       </c>
       <c r="M63">
         <f>$K$7/K63</f>
-        <v>2.0016474332986562</v>
+        <v>1.9511644782686504</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
@@ -1876,35 +1882,35 @@
         <v>2</v>
       </c>
       <c r="C64">
-        <v>1.5318999999999999E-2</v>
+        <v>0.25407299999999999</v>
       </c>
       <c r="D64">
-        <v>12.362632</v>
+        <v>247.52152699999999</v>
       </c>
       <c r="E64">
-        <f t="shared" ref="E64:E69" si="16">$C$7/C64</f>
-        <v>2.1206345061688103</v>
+        <f t="shared" ref="E64:E69" si="18">$C$7/C64</f>
+        <v>2.5475001279159928</v>
       </c>
       <c r="F64">
-        <f t="shared" ref="F64:F69" si="17">$D$7/D64</f>
-        <v>0.14458612049602385</v>
+        <f t="shared" ref="F64:F69" si="19">$D$7/D64</f>
+        <v>0.14249605045463379</v>
       </c>
       <c r="I64">
         <v>2</v>
       </c>
       <c r="J64">
-        <v>0.57489299999999999</v>
+        <v>0.193219</v>
       </c>
       <c r="K64">
-        <v>27.292974000000001</v>
+        <v>9.2611570000000007</v>
       </c>
       <c r="L64">
-        <f t="shared" ref="L64:L69" si="18">$J$7/J64</f>
-        <v>3.3955344733715669</v>
+        <f t="shared" ref="L64:L69" si="20">$J$7/J64</f>
+        <v>3.3686490459012828</v>
       </c>
       <c r="M64">
-        <f t="shared" ref="M64:M69" si="19">$K$7/K64</f>
-        <v>3.8837788802348912</v>
+        <f t="shared" ref="M64:M69" si="21">$K$7/K64</f>
+        <v>3.7720213575906332</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -1912,35 +1918,35 @@
         <v>4</v>
       </c>
       <c r="C65">
-        <v>1.2663000000000001E-2</v>
+        <v>0.18737899999999999</v>
       </c>
       <c r="D65">
-        <v>9.6678130000000007</v>
+        <v>205.26013</v>
       </c>
       <c r="E65">
-        <f t="shared" si="16"/>
-        <v>2.5654268340835507</v>
+        <f t="shared" si="18"/>
+        <v>3.4542344659753765</v>
       </c>
       <c r="F65">
-        <f t="shared" si="17"/>
-        <v>0.18488824721785579</v>
+        <f t="shared" si="19"/>
+        <v>0.17183483221997375</v>
       </c>
       <c r="I65">
         <v>4</v>
       </c>
       <c r="J65">
-        <v>0.44285400000000003</v>
+        <v>0.14974100000000001</v>
       </c>
       <c r="K65">
-        <v>15.512722</v>
+        <v>5.1284359999999998</v>
       </c>
       <c r="L65">
-        <f t="shared" si="18"/>
-        <v>4.4079290240124287</v>
+        <f t="shared" si="20"/>
+        <v>4.3467520585544372</v>
       </c>
       <c r="M65">
-        <f t="shared" si="19"/>
-        <v>6.8330932508169742</v>
+        <f t="shared" si="21"/>
+        <v>6.8116833280165725</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -1948,35 +1954,35 @@
         <v>8</v>
       </c>
       <c r="C66">
-        <v>1.2579999999999999E-2</v>
+        <v>0.16376099999999999</v>
       </c>
       <c r="D66">
-        <v>7.4328620000000001</v>
+        <v>151.23631599999999</v>
       </c>
       <c r="E66">
-        <f t="shared" si="16"/>
-        <v>2.5823529411764707</v>
+        <f t="shared" si="18"/>
+        <v>3.9524123570325052</v>
       </c>
       <c r="F66">
-        <f t="shared" si="17"/>
-        <v>0.24048139195911347</v>
+        <f t="shared" si="19"/>
+        <v>0.23321673611779861</v>
       </c>
       <c r="I66">
         <v>8</v>
       </c>
       <c r="J66">
-        <v>0.539941</v>
+        <v>0.150259</v>
       </c>
       <c r="K66">
-        <v>12.449930999999999</v>
+        <v>2.813663</v>
       </c>
       <c r="L66">
-        <f t="shared" si="18"/>
-        <v>3.6153376017009267</v>
+        <f t="shared" si="20"/>
+        <v>4.3317671487232046</v>
       </c>
       <c r="M66">
-        <f t="shared" si="19"/>
-        <v>8.5140934516022622</v>
+        <f t="shared" si="21"/>
+        <v>12.415588505091049</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -1984,35 +1990,35 @@
         <v>16</v>
       </c>
       <c r="C67">
-        <v>1.5805E-2</v>
+        <v>0.208287</v>
       </c>
       <c r="D67">
-        <v>5.2015000000000002</v>
+        <v>111.248386</v>
       </c>
       <c r="E67">
-        <f t="shared" si="16"/>
-        <v>2.0554254982600444</v>
+        <f t="shared" si="18"/>
+        <v>3.1074959070897368</v>
       </c>
       <c r="F67">
-        <f t="shared" si="17"/>
-        <v>0.34364414111314046</v>
+        <f t="shared" si="19"/>
+        <v>0.31704585808552765</v>
       </c>
       <c r="I67">
         <v>16</v>
       </c>
       <c r="J67">
-        <v>0.63332100000000002</v>
+        <v>0.20419499999999999</v>
       </c>
       <c r="K67">
-        <v>4.8977380000000004</v>
+        <v>1.524367</v>
       </c>
       <c r="L67">
-        <f t="shared" si="18"/>
-        <v>3.0822742337613942</v>
+        <f t="shared" si="20"/>
+        <v>3.1875756017532262</v>
       </c>
       <c r="M67">
-        <f t="shared" si="19"/>
-        <v>21.642618694589213</v>
+        <f t="shared" si="21"/>
+        <v>22.916582424048801</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
@@ -2020,35 +2026,35 @@
         <v>32</v>
       </c>
       <c r="C68">
-        <v>7.5187000000000004E-2</v>
+        <v>0.53544599999999998</v>
       </c>
       <c r="D68">
-        <v>4.7094240000000003</v>
+        <v>92.425984999999997</v>
       </c>
       <c r="E68">
-        <f t="shared" si="16"/>
-        <v>0.43206937369492066</v>
+        <f t="shared" si="18"/>
+        <v>1.2088072373311223</v>
       </c>
       <c r="F68">
-        <f t="shared" si="17"/>
-        <v>0.37955066267127358</v>
+        <f t="shared" si="19"/>
+        <v>0.38161172964507761</v>
       </c>
       <c r="I68">
         <v>32</v>
       </c>
       <c r="J68">
-        <v>1.131459</v>
+        <v>0.37990699999999999</v>
       </c>
       <c r="K68">
-        <v>3.8228179999999998</v>
+        <v>1.284457</v>
       </c>
       <c r="L68">
-        <f t="shared" si="18"/>
-        <v>1.725267110871892</v>
+        <f t="shared" si="20"/>
+        <v>1.7132798290107842</v>
       </c>
       <c r="M68">
-        <f t="shared" si="19"/>
-        <v>27.72820364453657</v>
+        <f t="shared" si="21"/>
+        <v>27.196926016207627</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
@@ -2056,35 +2062,35 @@
         <v>64</v>
       </c>
       <c r="C69">
-        <v>0.24757699999999999</v>
+        <v>1.0402629999999999</v>
       </c>
       <c r="D69">
-        <v>9.810962</v>
+        <v>104.83583900000001</v>
       </c>
       <c r="E69">
-        <f t="shared" si="16"/>
-        <v>0.13121574298097158</v>
+        <f t="shared" si="18"/>
+        <v>0.62219938611678016</v>
       </c>
       <c r="F69">
-        <f t="shared" si="17"/>
-        <v>0.18219059456147116</v>
+        <f t="shared" si="19"/>
+        <v>0.3364387630836817</v>
       </c>
       <c r="I69">
         <v>64</v>
       </c>
       <c r="J69">
-        <v>2.2527140000000001</v>
+        <v>0.73543599999999998</v>
       </c>
       <c r="K69">
-        <v>2.765174</v>
+        <v>0.87792099999999995</v>
       </c>
       <c r="L69">
-        <f t="shared" si="18"/>
-        <v>0.86654098123419132</v>
+        <f t="shared" si="20"/>
+        <v>0.88503554354151825</v>
       </c>
       <c r="M69">
-        <f t="shared" si="19"/>
-        <v>38.333890019217598</v>
+        <f t="shared" si="21"/>
+        <v>39.790917406008056</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
@@ -2095,18 +2101,18 @@
         <v>1</v>
       </c>
       <c r="C70">
-        <v>2.6328000000000001E-2</v>
+        <v>0.47770299999999999</v>
       </c>
       <c r="D70">
-        <v>9.7397109999999998</v>
+        <v>175.406014</v>
       </c>
       <c r="E70">
         <f>$C$14/C70</f>
-        <v>1.6535247645092679</v>
+        <v>1.7382829917333573</v>
       </c>
       <c r="F70">
         <f>$D$14/D70</f>
-        <v>0.12150576131057687</v>
+        <v>0.13256815128357</v>
       </c>
       <c r="H70">
         <v>0.5</v>
@@ -2115,18 +2121,18 @@
         <v>1</v>
       </c>
       <c r="J70">
-        <v>1.33674</v>
+        <v>0.453627</v>
       </c>
       <c r="K70">
-        <v>35.242871000000001</v>
+        <v>11.771865999999999</v>
       </c>
       <c r="L70">
         <f>$J$14/J70</f>
-        <v>1.8771189610545056</v>
+        <v>1.872412797298221</v>
       </c>
       <c r="M70">
         <f>$K$14/K70</f>
-        <v>1.9734019966761502</v>
+        <v>1.9629356127567201</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
@@ -2134,35 +2140,35 @@
         <v>2</v>
       </c>
       <c r="C71">
-        <v>1.7596000000000001E-2</v>
+        <v>0.30976999999999999</v>
       </c>
       <c r="D71">
-        <v>8.5071399999999997</v>
+        <v>172.10809</v>
       </c>
       <c r="E71">
-        <f t="shared" ref="E71:E76" si="20">$C$14/C71</f>
-        <v>2.4740850193225734</v>
+        <f t="shared" ref="E71:E76" si="22">$C$14/C71</f>
+        <v>2.6806437033928399</v>
       </c>
       <c r="F71">
-        <f t="shared" ref="F71:F76" si="21">$D$14/D71</f>
-        <v>0.13911032379859742</v>
+        <f t="shared" ref="F71:F76" si="23">$D$14/D71</f>
+        <v>0.13510841355569048</v>
       </c>
       <c r="I71">
         <v>2</v>
       </c>
       <c r="J71">
-        <v>0.717086</v>
+        <v>0.26731500000000002</v>
       </c>
       <c r="K71">
-        <v>18.357680999999999</v>
+        <v>6.688898</v>
       </c>
       <c r="L71">
-        <f t="shared" ref="L71:L76" si="22">$J$14/J71</f>
-        <v>3.4991897764005992</v>
+        <f t="shared" ref="L71:L76" si="24">$J$14/J71</f>
+        <v>3.17743860239792</v>
       </c>
       <c r="M71">
-        <f t="shared" ref="M71:M76" si="23">$K$14/K71</f>
-        <v>3.7885151180042835</v>
+        <f t="shared" ref="M71:M76" si="25">$K$14/K71</f>
+        <v>3.4545922213195657</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
@@ -2170,35 +2176,35 @@
         <v>4</v>
       </c>
       <c r="C72">
-        <v>1.3859E-2</v>
+        <v>0.22942399999999999</v>
       </c>
       <c r="D72">
-        <v>6.8628520000000002</v>
+        <v>136.11906099999999</v>
       </c>
       <c r="E72">
-        <f t="shared" si="20"/>
-        <v>3.1412078793563754</v>
+        <f t="shared" si="22"/>
+        <v>3.6194251691191854</v>
       </c>
       <c r="F72">
-        <f t="shared" si="21"/>
-        <v>0.17244011673281018</v>
+        <f t="shared" si="23"/>
+        <v>0.17083023368784481</v>
       </c>
       <c r="I72">
         <v>4</v>
       </c>
       <c r="J72">
-        <v>0.53298900000000005</v>
+        <v>0.18276000000000001</v>
       </c>
       <c r="K72">
-        <v>10.200006</v>
+        <v>3.5629110000000002</v>
       </c>
       <c r="L72">
-        <f t="shared" si="22"/>
-        <v>4.7078269908009354</v>
+        <f t="shared" si="24"/>
+        <v>4.6474994528343183</v>
       </c>
       <c r="M72">
-        <f t="shared" si="23"/>
-        <v>6.8184618714930165</v>
+        <f t="shared" si="25"/>
+        <v>6.4855437028878908</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
@@ -2206,35 +2212,35 @@
         <v>8</v>
       </c>
       <c r="C73">
-        <v>1.4121E-2</v>
+        <v>0.17718</v>
       </c>
       <c r="D73">
-        <v>4.8270869999999997</v>
+        <v>95.165251999999995</v>
       </c>
       <c r="E73">
-        <f t="shared" si="20"/>
-        <v>3.0829261383754694</v>
+        <f t="shared" si="22"/>
+        <v>4.6866632802799408</v>
       </c>
       <c r="F73">
-        <f t="shared" si="21"/>
-        <v>0.24516463034538222</v>
+        <f t="shared" si="23"/>
+        <v>0.24434602453424911</v>
       </c>
       <c r="I73">
         <v>8</v>
       </c>
       <c r="J73">
-        <v>0.50183599999999995</v>
+        <v>0.162767</v>
       </c>
       <c r="K73">
-        <v>5.8779440000000003</v>
+        <v>1.8700950000000001</v>
       </c>
       <c r="L73">
-        <f t="shared" si="22"/>
-        <v>5.0000797073147405</v>
+        <f t="shared" si="24"/>
+        <v>5.2183612157255466</v>
       </c>
       <c r="M73">
-        <f t="shared" si="23"/>
-        <v>11.832088226767725</v>
+        <f t="shared" si="25"/>
+        <v>12.356278691724217</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -2242,35 +2248,35 @@
         <v>16</v>
       </c>
       <c r="C74">
-        <v>2.0421000000000002E-2</v>
+        <v>0.24124499999999999</v>
       </c>
       <c r="D74">
-        <v>3.5760930000000002</v>
+        <v>73.173834999999997</v>
       </c>
       <c r="E74">
-        <f t="shared" si="20"/>
-        <v>2.1318250820234073</v>
+        <f t="shared" si="22"/>
+        <v>3.4420734108478932</v>
       </c>
       <c r="F74">
-        <f t="shared" si="21"/>
-        <v>0.33092847417558768</v>
+        <f t="shared" si="23"/>
+        <v>0.31778095271349383</v>
       </c>
       <c r="I74">
         <v>16</v>
       </c>
       <c r="J74">
-        <v>0.65846300000000002</v>
+        <v>0.21198900000000001</v>
       </c>
       <c r="K74">
-        <v>3.389507</v>
+        <v>1.0211600000000001</v>
       </c>
       <c r="L74">
-        <f t="shared" si="22"/>
-        <v>3.8107228500310573</v>
+        <f t="shared" si="24"/>
+        <v>4.0067031779950844</v>
       </c>
       <c r="M74">
-        <f t="shared" si="23"/>
-        <v>20.518722044238292</v>
+        <f t="shared" si="25"/>
+        <v>22.628593951976182</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
@@ -2278,35 +2284,35 @@
         <v>32</v>
       </c>
       <c r="C75">
-        <v>0.121341</v>
+        <v>0.42706100000000002</v>
       </c>
       <c r="D75">
-        <v>3.4536639999999998</v>
+        <v>61.885283999999999</v>
       </c>
       <c r="E75">
-        <f t="shared" si="20"/>
-        <v>0.35877403350887171</v>
+        <f t="shared" si="22"/>
+        <v>1.9444130932115082</v>
       </c>
       <c r="F75">
-        <f t="shared" si="21"/>
-        <v>0.34265956387187635</v>
+        <f t="shared" si="23"/>
+        <v>0.37574766563243045</v>
       </c>
       <c r="I75">
         <v>32</v>
       </c>
       <c r="J75">
-        <v>1.1885810000000001</v>
+        <v>0.39147399999999999</v>
       </c>
       <c r="K75">
-        <v>2.7266189999999999</v>
+        <v>0.89611200000000002</v>
       </c>
       <c r="L75">
-        <f t="shared" si="22"/>
-        <v>2.1111055956640734</v>
+        <f t="shared" si="24"/>
+        <v>2.1696894302048157</v>
       </c>
       <c r="M75">
-        <f t="shared" si="23"/>
-        <v>25.507176470199905</v>
+        <f t="shared" si="25"/>
+        <v>25.786302381845125</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
@@ -2314,35 +2320,35 @@
         <v>64</v>
       </c>
       <c r="C76">
-        <v>0.14918000000000001</v>
+        <v>1.0753729999999999</v>
       </c>
       <c r="D76">
-        <v>10.280018999999999</v>
+        <v>71.866376000000002</v>
       </c>
       <c r="E76">
-        <f t="shared" si="20"/>
-        <v>0.29182196004826383</v>
+        <f t="shared" si="22"/>
+        <v>0.77218137334673653</v>
       </c>
       <c r="F76">
-        <f t="shared" si="21"/>
-        <v>0.11511953431214475</v>
+        <f t="shared" si="23"/>
+        <v>0.32356231514999445</v>
       </c>
       <c r="I76">
         <v>64</v>
       </c>
       <c r="J76">
-        <v>2.3766440000000002</v>
+        <v>0.64367700000000005</v>
       </c>
       <c r="K76">
-        <v>2.235096</v>
+        <v>0.63083800000000001</v>
       </c>
       <c r="L76">
-        <f t="shared" si="22"/>
-        <v>1.0557828602011912</v>
+        <f t="shared" si="24"/>
+        <v>1.3195702192248597</v>
       </c>
       <c r="M76">
-        <f t="shared" si="23"/>
-        <v>31.116494325075969</v>
+        <f t="shared" si="25"/>
+        <v>36.629713175173343</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
@@ -2353,18 +2359,18 @@
         <v>1</v>
       </c>
       <c r="C77">
-        <v>2.4390999999999999E-2</v>
+        <v>0.38083899999999998</v>
       </c>
       <c r="D77">
-        <v>5.7500590000000003</v>
+        <v>116.514312</v>
       </c>
       <c r="E77">
         <f>$C$21/C77</f>
-        <v>1.3166331843712844</v>
+        <v>1.7124270360966185</v>
       </c>
       <c r="F77">
         <f>$D$21/D77</f>
-        <v>0.1001687113123535</v>
+        <v>9.9581611913908061E-2</v>
       </c>
       <c r="H77">
         <v>0.75</v>
@@ -2373,18 +2379,18 @@
         <v>1</v>
       </c>
       <c r="J77">
-        <v>1.023892</v>
+        <v>0.34847600000000001</v>
       </c>
       <c r="K77">
-        <v>17.332422000000001</v>
+        <v>5.8378319999999997</v>
       </c>
       <c r="L77">
         <f>$J$21/J77</f>
-        <v>1.8851548796162096</v>
+        <v>1.8729123382958943</v>
       </c>
       <c r="M77">
         <f>$K$21/K77</f>
-        <v>2.0232740121374841</v>
+        <v>1.9758143091476423</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
@@ -2392,35 +2398,35 @@
         <v>2</v>
       </c>
       <c r="C78">
-        <v>1.6115000000000001E-2</v>
+        <v>0.25404700000000002</v>
       </c>
       <c r="D78">
-        <v>4.4530750000000001</v>
+        <v>96.670518000000001</v>
       </c>
       <c r="E78">
-        <f t="shared" ref="E78:E83" si="24">$C$21/C78</f>
-        <v>1.9928017375116349</v>
+        <f t="shared" ref="E78:E83" si="26">$C$21/C78</f>
+        <v>2.5670801072242537</v>
       </c>
       <c r="F78">
-        <f t="shared" ref="F78:F83" si="25">$D$21/D78</f>
-        <v>0.12934343122449093</v>
+        <f t="shared" ref="F78:F83" si="27">$D$21/D78</f>
+        <v>0.12002297329160894</v>
       </c>
       <c r="I78">
         <v>2</v>
       </c>
       <c r="J78">
-        <v>0.56249700000000002</v>
+        <v>0.189556</v>
       </c>
       <c r="K78">
-        <v>9.3536780000000004</v>
+        <v>3.2981229999999999</v>
       </c>
       <c r="L78">
-        <f t="shared" ref="L78:L83" si="26">$J$21/J78</f>
-        <v>3.4314760789835326</v>
+        <f t="shared" ref="L78:L83" si="28">$J$21/J78</f>
+        <v>3.4431249868112856</v>
       </c>
       <c r="M78">
-        <f t="shared" ref="M78:M83" si="27">$K$21/K78</f>
-        <v>3.7491390017915944</v>
+        <f t="shared" ref="M78:M83" si="29">$K$21/K78</f>
+        <v>3.4972837580648144</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
@@ -2428,35 +2434,35 @@
         <v>4</v>
       </c>
       <c r="C79">
-        <v>1.2274999999999999E-2</v>
+        <v>0.18048</v>
       </c>
       <c r="D79">
-        <v>3.8394140000000001</v>
+        <v>76.878956000000002</v>
       </c>
       <c r="E79">
-        <f t="shared" si="24"/>
-        <v>2.6162118126272911</v>
+        <f t="shared" si="26"/>
+        <v>3.6134696365248229</v>
       </c>
       <c r="F79">
-        <f t="shared" si="25"/>
-        <v>0.1500166431648163</v>
+        <f t="shared" si="27"/>
+        <v>0.15092144331408455</v>
       </c>
       <c r="I79">
         <v>4</v>
       </c>
       <c r="J79">
-        <v>0.45862599999999998</v>
+        <v>0.15434400000000001</v>
       </c>
       <c r="K79">
-        <v>5.2896219999999996</v>
+        <v>1.7318480000000001</v>
       </c>
       <c r="L79">
-        <f t="shared" si="26"/>
-        <v>4.20864713295801</v>
+        <f t="shared" si="28"/>
+        <v>4.2286386254081796</v>
       </c>
       <c r="M79">
-        <f t="shared" si="27"/>
-        <v>6.6296304348401458</v>
+        <f t="shared" si="29"/>
+        <v>6.6602103648819062</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
@@ -2464,35 +2470,35 @@
         <v>8</v>
       </c>
       <c r="C80">
-        <v>1.0841999999999999E-2</v>
+        <v>0.15826499999999999</v>
       </c>
       <c r="D80">
-        <v>2.6904379999999999</v>
+        <v>55.569130999999999</v>
       </c>
       <c r="E80">
-        <f t="shared" si="24"/>
-        <v>2.961999631064379</v>
+        <f t="shared" si="26"/>
+        <v>4.1206773449594039</v>
       </c>
       <c r="F80">
-        <f t="shared" si="25"/>
-        <v>0.21408261405763673</v>
+        <f t="shared" si="27"/>
+        <v>0.20879727271603368</v>
       </c>
       <c r="I80">
         <v>8</v>
       </c>
       <c r="J80">
-        <v>0.44102200000000003</v>
+        <v>0.15176700000000001</v>
       </c>
       <c r="K80">
-        <v>2.9059140000000001</v>
+        <v>0.91381599999999996</v>
       </c>
       <c r="L80">
-        <f t="shared" si="26"/>
-        <v>4.376641074594918</v>
+        <f t="shared" si="28"/>
+        <v>4.3004408072901219</v>
       </c>
       <c r="M80">
-        <f t="shared" si="27"/>
-        <v>12.067886042050796</v>
+        <f t="shared" si="29"/>
+        <v>12.622313463541895</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
@@ -2500,35 +2506,35 @@
         <v>16</v>
       </c>
       <c r="C81">
-        <v>1.6619999999999999E-2</v>
+        <v>0.25487300000000002</v>
       </c>
       <c r="D81">
-        <v>1.9562029999999999</v>
+        <v>41.562624</v>
       </c>
       <c r="E81">
-        <f t="shared" si="24"/>
-        <v>1.9322503008423584</v>
+        <f t="shared" si="26"/>
+        <v>2.5587606376509084</v>
       </c>
       <c r="F81">
-        <f t="shared" si="25"/>
-        <v>0.29443570018040055</v>
+        <f t="shared" si="27"/>
+        <v>0.27916146487767474</v>
       </c>
       <c r="I81">
         <v>16</v>
       </c>
       <c r="J81">
-        <v>0.638903</v>
+        <v>0.206235</v>
       </c>
       <c r="K81">
-        <v>1.8532759999999999</v>
+        <v>0.57039499999999999</v>
       </c>
       <c r="L81">
-        <f t="shared" si="26"/>
-        <v>3.021108055526426</v>
+        <f t="shared" si="28"/>
+        <v>3.1646665212015423</v>
       </c>
       <c r="M81">
-        <f t="shared" si="27"/>
-        <v>18.922297056671539</v>
+        <f t="shared" si="29"/>
+        <v>20.221902365904327</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -2536,35 +2542,35 @@
         <v>32</v>
       </c>
       <c r="C82">
-        <v>0.114021</v>
+        <v>0.43500499999999998</v>
       </c>
       <c r="D82">
-        <v>2.2744559999999998</v>
+        <v>37.427360999999998</v>
       </c>
       <c r="E82">
-        <f t="shared" si="24"/>
-        <v>0.28164987151489634</v>
+        <f t="shared" si="26"/>
+        <v>1.4991988597832211</v>
       </c>
       <c r="F82">
-        <f t="shared" si="25"/>
-        <v>0.25323681794679698</v>
+        <f t="shared" si="27"/>
+        <v>0.31000537280734275</v>
       </c>
       <c r="I82">
         <v>32</v>
       </c>
       <c r="J82">
-        <v>1.2797559999999999</v>
+        <v>0.41375400000000001</v>
       </c>
       <c r="K82">
-        <v>1.7206509999999999</v>
+        <v>0.50070800000000004</v>
       </c>
       <c r="L82">
-        <f t="shared" si="26"/>
-        <v>1.5082523543550492</v>
+        <f t="shared" si="28"/>
+        <v>1.5774228164561552</v>
       </c>
       <c r="M82">
-        <f t="shared" si="27"/>
-        <v>20.380797151775695</v>
+        <f t="shared" si="29"/>
+        <v>23.036324564416784</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
@@ -2572,48 +2578,48 @@
         <v>64</v>
       </c>
       <c r="C83">
-        <v>0.39291199999999998</v>
+        <v>1.1214139999999999</v>
       </c>
       <c r="D83">
-        <v>10.721268999999999</v>
+        <v>44.177781000000003</v>
       </c>
       <c r="E83">
-        <f t="shared" si="24"/>
-        <v>8.1733314329926282E-2</v>
+        <f t="shared" si="26"/>
+        <v>0.5815506137786759</v>
       </c>
       <c r="F83">
-        <f t="shared" si="25"/>
-        <v>5.3722744947449788E-2</v>
+        <f t="shared" si="27"/>
+        <v>0.26263616545158752</v>
       </c>
       <c r="I83">
         <v>64</v>
       </c>
       <c r="J83">
-        <v>2.4354580000000001</v>
+        <v>0.74003200000000002</v>
       </c>
       <c r="K83">
-        <v>1.803477</v>
+        <v>0.43029600000000001</v>
       </c>
       <c r="L83">
-        <f t="shared" si="26"/>
-        <v>0.79253881610768895</v>
+        <f t="shared" si="28"/>
+        <v>0.8819415917149529</v>
       </c>
       <c r="M83">
-        <f t="shared" si="27"/>
-        <v>19.444794139320877</v>
+        <f t="shared" si="29"/>
+        <v>26.805901054158067</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D85" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C86" t="s">
         <v>4</v>
@@ -2669,11 +2675,11 @@
         <v>2.1765340000000002</v>
       </c>
       <c r="E89">
-        <f t="shared" ref="E89:E94" si="28">$C$33/C89</f>
+        <f t="shared" ref="E89:E94" si="30">$C$33/C89</f>
         <v>0.59446052087639523</v>
       </c>
       <c r="F89">
-        <f t="shared" ref="F89:F94" si="29">$D$33/D89</f>
+        <f t="shared" ref="F89:F94" si="31">$D$33/D89</f>
         <v>0.12669041696568947</v>
       </c>
     </row>
@@ -2688,11 +2694,11 @@
         <v>1.7092799999999999</v>
       </c>
       <c r="E90">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>0.5075891281327215</v>
       </c>
       <c r="F90">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.16132289619020876</v>
       </c>
     </row>
@@ -2707,11 +2713,11 @@
         <v>1.1646259999999999</v>
       </c>
       <c r="E91">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>0.44547707558859978</v>
       </c>
       <c r="F91">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.23676785508824291</v>
       </c>
     </row>
@@ -2726,11 +2732,11 @@
         <v>0.836009</v>
       </c>
       <c r="E92">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>0.26765937645416477</v>
       </c>
       <c r="F92">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.32983616205088701</v>
       </c>
     </row>
@@ -2745,11 +2751,11 @@
         <v>1.0019910000000001</v>
       </c>
       <c r="E93">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>0.12349708004122295</v>
       </c>
       <c r="F93">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.2751980806214826</v>
       </c>
     </row>
@@ -2764,11 +2770,11 @@
         <v>4.1503180000000004</v>
       </c>
       <c r="E94">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>8.3478462788807613E-3</v>
       </c>
       <c r="F94">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>6.6439728232872752E-2</v>
       </c>
     </row>
@@ -2805,11 +2811,11 @@
         <v>8.5071399999999997</v>
       </c>
       <c r="E96">
-        <f t="shared" ref="E96:E101" si="30">$C$40/C96</f>
+        <f t="shared" ref="E96:E101" si="32">$C$40/C96</f>
         <v>2.4740850193225734</v>
       </c>
       <c r="F96">
-        <f t="shared" ref="F96:F101" si="31">$D$40/D96</f>
+        <f t="shared" ref="F96:F101" si="33">$D$40/D96</f>
         <v>0.13911032379859742</v>
       </c>
     </row>
@@ -2824,11 +2830,11 @@
         <v>6.8628520000000002</v>
       </c>
       <c r="E97">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>3.1412078793563754</v>
       </c>
       <c r="F97">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.17244011673281018</v>
       </c>
     </row>
@@ -2843,11 +2849,11 @@
         <v>4.8270869999999997</v>
       </c>
       <c r="E98">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>3.0829261383754694</v>
       </c>
       <c r="F98">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.24516463034538222</v>
       </c>
     </row>
@@ -2862,11 +2868,11 @@
         <v>3.5760930000000002</v>
       </c>
       <c r="E99">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>2.1318250820234073</v>
       </c>
       <c r="F99">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.33092847417558768</v>
       </c>
     </row>
@@ -2881,11 +2887,11 @@
         <v>3.4536639999999998</v>
       </c>
       <c r="E100">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.35877403350887171</v>
       </c>
       <c r="F100">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.34265956387187635</v>
       </c>
     </row>
@@ -2900,17 +2906,17 @@
         <v>10.280018999999999</v>
       </c>
       <c r="E101">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.29182196004826383</v>
       </c>
       <c r="F101">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.11511953431214475</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C102" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -2946,11 +2952,11 @@
         <v>1.906237</v>
       </c>
       <c r="E104">
-        <f t="shared" ref="E104:E109" si="32">$C$48/C104</f>
+        <f t="shared" ref="E104:E109" si="34">$C$48/C104</f>
         <v>3.0412284998127288</v>
       </c>
       <c r="F104">
-        <f t="shared" ref="F104:F109" si="33">$D$48/D104</f>
+        <f t="shared" ref="F104:F109" si="35">$D$48/D104</f>
         <v>0.15408367375095541</v>
       </c>
     </row>
@@ -2965,11 +2971,11 @@
         <v>1.5417339999999999</v>
       </c>
       <c r="E105">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>5.3894618605126112</v>
       </c>
       <c r="F105">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.19051276030754979</v>
       </c>
     </row>
@@ -2984,11 +2990,11 @@
         <v>1.1164480000000001</v>
       </c>
       <c r="E106">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>10.275284726954153</v>
       </c>
       <c r="F106">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.26308435323454382</v>
       </c>
     </row>
@@ -3003,11 +3009,11 @@
         <v>0.87336400000000003</v>
       </c>
       <c r="E107">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>11.4500488122356</v>
       </c>
       <c r="F107">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.33630880137033353</v>
       </c>
     </row>
@@ -3022,11 +3028,11 @@
         <v>0.94589400000000001</v>
       </c>
       <c r="E108">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>2.866943697547462</v>
       </c>
       <c r="F108">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.31052105204177211</v>
       </c>
     </row>
@@ -3041,11 +3047,11 @@
         <v>4.0405769999999999</v>
       </c>
       <c r="E109">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>0.31438246620384025</v>
       </c>
       <c r="F109">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>7.2692588212030118E-2</v>
       </c>
     </row>

</xml_diff>